<commit_message>
added commond string lookup file, cleaned up reader and added val lookup for string
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkisf\Desktop\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkisf\Desktop\Python101\Git_PydPiper\pylightxl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6B2EB5-80F6-4C77-A2A0-6069DE23B2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5429558-3DE9-458D-A372-99EC3A0AD419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29700" yWindow="3060" windowWidth="11160" windowHeight="10335" xr2:uid="{22B1298B-A9E3-476A-B9AD-473AE2D00811}"/>
   </bookViews>
@@ -32,9 +32,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +405,7 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>10</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,20 +418,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>3</f>
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>30</v>
+      <c r="B3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <f>A1+10</f>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
+      <c r="A5" t="str">
+        <f>"this"&amp;A2</f>
+        <v>thistwo</v>
       </c>
     </row>
   </sheetData>
@@ -438,7 +447,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,8 +473,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>200</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>